<commit_message>
Switch to permanent PostgreSQL
</commit_message>
<xml_diff>
--- a/exports/SouthernLabs_MCC_Week_1.xlsx
+++ b/exports/SouthernLabs_MCC_Week_1.xlsx
@@ -459,14 +459,14 @@
   <sheetData>
     <row r="1"/>
     <row r="2">
-      <c r="C2" s="1" t="inlineStr">
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>Southern Labs Institute of Technology</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="2" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>Attendance Report: MCC - Week 1</t>
         </is>

</xml_diff>